<commit_message>
Second commit, still unorganized
</commit_message>
<xml_diff>
--- a/Accuracy Results.xlsx
+++ b/Accuracy Results.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Andree/Dropbox/My Mac (Macbooks-MacBook-Pro.local)/Desktop/occupacny_detection/dataset-cleaning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Andree/Dropbox/My Mac (Macbooks-MacBook-Pro.local)/Desktop/occupacny_detection/experimentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7FC5CA-FDD7-2241-9FAD-10453F3F2250}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EAF5D6-A12F-054D-9DF9-153C326DAB6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{48E0AA12-B65A-DE4A-8794-21F6F44F596D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{48E0AA12-B65A-DE4A-8794-21F6F44F596D}"/>
   </bookViews>
   <sheets>
     <sheet name="Gym_v2" sheetId="3" r:id="rId1"/>
-    <sheet name="Gym" sheetId="1" r:id="rId2"/>
-    <sheet name="Dressing Room" sheetId="2" r:id="rId3"/>
+    <sheet name="Dressing_Room_v2" sheetId="4" r:id="rId2"/>
+    <sheet name="Residential" sheetId="5" r:id="rId3"/>
+    <sheet name="Gym" sheetId="1" r:id="rId4"/>
+    <sheet name="Dressing Room" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="33">
   <si>
     <t>SVM</t>
   </si>
@@ -88,12 +90,51 @@
   <si>
     <t>There were only 9 test instances, so 2 errors significantly affected the precision</t>
   </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>5 minutes dataset had only 15 instances</t>
+  </si>
+  <si>
+    <t>1 minute dataset had 66 instances</t>
+  </si>
+  <si>
+    <t>SVC Learning Curves</t>
+  </si>
+  <si>
+    <t>KNN Learning Curves</t>
+  </si>
+  <si>
+    <t>DT Learning Curves</t>
+  </si>
+  <si>
+    <t>Learning Curves SVC</t>
+  </si>
+  <si>
+    <t>Learning Curves KNN</t>
+  </si>
+  <si>
+    <t>SVM took. 4:17 hours to complete the grid search with the last three datasets. The search was reduced to only RBF Kernel, and it tooks allways both values of gamma and C as 10, as optimal parameters. We must test increasing these values.</t>
+  </si>
+  <si>
+    <t>DT took 27 minutes to complete the grid seach with all the datasets. It is portant to stress that it allways took the max_depth available (12) and criterion gini as optimal parameters . We must test is increasing this parameters has a positive effect on the accuracy.</t>
+  </si>
+  <si>
+    <t>Decision Trees</t>
+  </si>
+  <si>
+    <t>10 sec avg.</t>
+  </si>
+  <si>
+    <t>10 sec avg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -129,8 +170,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,6 +215,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -186,10 +239,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -210,8 +264,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,12 +289,18 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -250,16 +320,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>394801</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>22700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>339402</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>74778</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>339403</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>58600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -311,16 +381,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>304643</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>23092</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>346470</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>130849</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>322202</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114671</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -370,10 +440,508 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>824502</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>18795</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76863F22-AD6D-A040-B81E-42F51DF6246C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="3672485"/>
+          <a:ext cx="5751401" cy="4063380"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>784649</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>88981</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>31186</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>113249</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D12B7814-0F3D-224C-B157-2C88A0A97024}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6536050" y="3761465"/>
+          <a:ext cx="5847302" cy="4068854"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>64714</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>8741</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F33D82CB-4934-0340-B8D0-2DF840DE06E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="8121529"/>
+          <a:ext cx="5816115" cy="4053327"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>800828</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>56624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>10989</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>100326</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{532A7EDB-2413-1B46-85E4-EA7C2C72B7F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="800828" y="3810000"/>
+          <a:ext cx="5786658" cy="4088288"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>825095</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>4181</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>16179</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43A30305-D24E-294B-B83C-BDDF69BB42D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7401592" y="3753377"/>
+          <a:ext cx="5779850" cy="4060764"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>8089</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>1583</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76CDFD60-2630-954C-B154-28F496F6EA8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="825097" y="8404650"/>
+          <a:ext cx="5759489" cy="4046169"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>94435</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>7285</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>102133</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1168440B-A899-4D4A-9734-89907262B997}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1" y="11817512"/>
+          <a:ext cx="13032925" cy="6846159"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>70273</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>18955</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>18236</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A568AE08-81C3-0A49-8772-9BCD6915AF13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="3587196"/>
+          <a:ext cx="13044596" cy="7567963"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -500,7 +1068,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -863,10 +1431,514 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{162D04C0-E2EE-B942-883E-0ED821A2F1B7}">
-  <dimension ref="A1:P29"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A16" zoomScale="164" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+    </row>
+    <row r="2" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+    </row>
+    <row r="3" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>0.99921000000000004</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0.91427999999999998</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4">
+        <v>0.99921000000000004</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0.91427999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0.99921000000000004</v>
+      </c>
+      <c r="D5">
+        <v>0.99573999999999996</v>
+      </c>
+      <c r="E5">
+        <v>0.93095000000000006</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0.99921000000000004</v>
+      </c>
+      <c r="H5">
+        <v>0.98704000000000003</v>
+      </c>
+      <c r="I5">
+        <v>0.94760999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="12">
+        <v>1</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0.99804000000000004</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.98931000000000002</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0.89641999999999999</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0.99948999999999999</v>
+      </c>
+      <c r="G6" s="12">
+        <v>0.99529999999999996</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0.98487000000000002</v>
+      </c>
+      <c r="I6" s="12">
+        <v>0.90595000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="8">
+        <f>AVERAGE(B4:B6)</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="8">
+        <f t="shared" ref="C7:I7" si="0">AVERAGE(C4:C6)</f>
+        <v>0.99881999999999993</v>
+      </c>
+      <c r="D7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.99501666666666677</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.91388333333333327</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.99974499999999999</v>
+      </c>
+      <c r="G7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.99790666666666672</v>
+      </c>
+      <c r="H7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.99063666666666661</v>
+      </c>
+      <c r="I7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.92261333333333317</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+    </row>
+    <row r="10" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+    </row>
+    <row r="11" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>0.99507000000000001</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0.88888</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12">
+        <v>0.99507000000000001</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0.88888</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+    </row>
+    <row r="13" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0.99507000000000001</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0.77776999999999996</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0.99507000000000001</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0.88888</v>
+      </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+    </row>
+    <row r="14" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="12">
+        <v>1</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0.99507000000000001</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0.97221999999999997</v>
+      </c>
+      <c r="E14" s="12">
+        <v>0.77776999999999996</v>
+      </c>
+      <c r="F14" s="12">
+        <v>0.99802000000000002</v>
+      </c>
+      <c r="G14" s="12">
+        <v>0.98521999999999998</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0.97221999999999997</v>
+      </c>
+      <c r="I14" s="12">
+        <v>0.77776999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ref="B15:I15" si="1">AVERAGE(B12:B14)</f>
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>0.99507000000000001</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>0.99074000000000007</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>0.81480666666666668</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0.99900999999999995</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0.99178666666666671</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>0.99074000000000007</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0.8518433333333334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="15"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="J12:Q12"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="I18:O18"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:I10"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B7:I7">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:I6">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11:I14 A16">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:I15">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55BC68BF-613A-EF40-A946-956E27C254E2}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:P59"/>
+  <sheetViews>
+    <sheetView topLeftCell="B12" zoomScale="180" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -875,17 +1947,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
@@ -895,19 +1967,19 @@
       <c r="P1" s="10"/>
     </row>
     <row r="2" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
@@ -954,26 +2026,26 @@
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4">
-        <v>0.99921000000000004</v>
+      <c r="C4" s="1">
+        <v>0.99914000000000003</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>0.91427999999999998</v>
+      <c r="E4" t="s">
+        <v>16</v>
       </c>
       <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="G4">
-        <v>0.99921000000000004</v>
+      <c r="G4" s="1">
+        <v>0.99914000000000003</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4">
-        <v>0.91427999999999998</v>
+      <c r="I4" t="s">
+        <v>16</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
@@ -989,26 +2061,26 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5">
-        <v>0.99921000000000004</v>
+      <c r="C5" s="1">
+        <v>0.99956999999999996</v>
       </c>
       <c r="D5">
-        <v>0.99573999999999996</v>
-      </c>
-      <c r="E5">
-        <v>0.93095000000000006</v>
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5">
-        <v>0.99921000000000004</v>
+      <c r="G5" s="1">
+        <v>0.99914000000000003</v>
       </c>
       <c r="H5">
-        <v>0.98704000000000003</v>
-      </c>
-      <c r="I5">
-        <v>0.94760999999999995</v>
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
@@ -1017,33 +2089,33 @@
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
     </row>
-    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="17">
-        <v>1</v>
-      </c>
-      <c r="C6" s="17">
-        <v>0.99804000000000004</v>
-      </c>
-      <c r="D6" s="17">
-        <v>0.98931000000000002</v>
-      </c>
-      <c r="E6" s="17">
-        <v>0.89641999999999999</v>
-      </c>
-      <c r="F6" s="17">
-        <v>0.99948999999999999</v>
-      </c>
-      <c r="G6" s="17">
-        <v>0.99529999999999996</v>
-      </c>
-      <c r="H6" s="17">
-        <v>0.98487000000000002</v>
-      </c>
-      <c r="I6" s="17">
-        <v>0.90595000000000003</v>
+      <c r="B6" s="14">
+        <v>0.99978</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0.99485999999999997</v>
+      </c>
+      <c r="D6" s="12">
+        <v>1</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0.99956999999999996</v>
+      </c>
+      <c r="G6" s="14">
+        <v>0.99570000000000003</v>
+      </c>
+      <c r="H6" s="12">
+        <v>1</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.25">
@@ -1052,36 +2124,30 @@
       </c>
       <c r="B7" s="8">
         <f>AVERAGE(B4:B6)</f>
-        <v>1</v>
+        <v>0.99988999999999995</v>
       </c>
       <c r="C7" s="8">
-        <f t="shared" ref="C7:I7" si="0">AVERAGE(C4:C6)</f>
-        <v>0.99881999999999993</v>
+        <f t="shared" ref="C7:H7" si="0">AVERAGE(C4:C6)</f>
+        <v>0.99785666666666673</v>
       </c>
       <c r="D7" s="8">
         <f t="shared" si="0"/>
-        <v>0.99501666666666677</v>
-      </c>
-      <c r="E7" s="8">
-        <f t="shared" si="0"/>
-        <v>0.91388333333333327</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E7" s="8"/>
       <c r="F7" s="8">
         <f t="shared" si="0"/>
-        <v>0.99974499999999999</v>
+        <v>0.99978499999999992</v>
       </c>
       <c r="G7" s="8">
         <f t="shared" si="0"/>
-        <v>0.99790666666666672</v>
+        <v>0.9979933333333334</v>
       </c>
       <c r="H7" s="8">
         <f t="shared" si="0"/>
-        <v>0.99063666666666661</v>
-      </c>
-      <c r="I7" s="8">
-        <f t="shared" si="0"/>
-        <v>0.92261333333333317</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I7" s="8"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
@@ -1103,17 +2169,17 @@
       <c r="O8" s="10"/>
     </row>
     <row r="9" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
@@ -1122,19 +2188,19 @@
       <c r="O9" s="10"/>
     </row>
     <row r="10" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="15" t="s">
+      <c r="A10" s="11"/>
+      <c r="B10" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16" t="s">
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
@@ -1168,7 +2234,9 @@
         <v>14</v>
       </c>
       <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
+      <c r="K11" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
@@ -1182,28 +2250,30 @@
         <v>16</v>
       </c>
       <c r="C12">
-        <v>0.99507000000000001</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12">
-        <v>0.88888</v>
+      <c r="E12" t="s">
+        <v>16</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
       </c>
       <c r="G12">
-        <v>0.99507000000000001</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="I12">
-        <v>0.88888</v>
+      <c r="I12" t="s">
+        <v>16</v>
       </c>
       <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
+      <c r="K12" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
@@ -1217,25 +2287,25 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>0.99507000000000001</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13">
-        <v>0.77776999999999996</v>
+      <c r="E13" t="s">
+        <v>16</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13">
-        <v>0.99507000000000001</v>
+        <v>1</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
-      <c r="I13">
-        <v>0.88888</v>
+      <c r="I13" t="s">
+        <v>16</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -1244,33 +2314,33 @@
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
     </row>
-    <row r="14" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="17">
-        <v>1</v>
-      </c>
-      <c r="C14" s="17">
+      <c r="B14" s="14">
+        <v>0.99950000000000006</v>
+      </c>
+      <c r="C14" s="14">
         <v>0.99507000000000001</v>
       </c>
-      <c r="D14" s="17">
-        <v>0.97221999999999997</v>
-      </c>
-      <c r="E14" s="17">
-        <v>0.77776999999999996</v>
-      </c>
-      <c r="F14" s="17">
-        <v>0.99802000000000002</v>
-      </c>
-      <c r="G14" s="17">
-        <v>0.98521999999999998</v>
-      </c>
-      <c r="H14" s="17">
-        <v>0.97221999999999997</v>
-      </c>
-      <c r="I14" s="17">
-        <v>0.77776999999999996</v>
+      <c r="D14" s="12">
+        <v>1</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="12">
+        <v>1</v>
+      </c>
+      <c r="G14" s="14">
+        <v>0.99507000000000001</v>
+      </c>
+      <c r="H14" s="12">
+        <v>1</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
@@ -1279,96 +2349,141 @@
       </c>
       <c r="B15">
         <f>AVERAGE(B12:B14)</f>
-        <v>1</v>
+        <v>0.99975000000000003</v>
       </c>
       <c r="C15">
         <f>AVERAGE(C12:C14)</f>
-        <v>0.99507000000000001</v>
+        <v>0.99835666666666667</v>
       </c>
       <c r="D15">
-        <f>AVERAGE(D12:D14)</f>
-        <v>0.99074000000000007</v>
-      </c>
-      <c r="E15">
-        <f>AVERAGE(E12:E14)</f>
-        <v>0.81480666666666668</v>
+        <f t="shared" ref="D15:H15" si="1">AVERAGE(D12:D14)</f>
+        <v>1</v>
       </c>
       <c r="F15">
-        <f>AVERAGE(F12:F14)</f>
-        <v>0.99900999999999995</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="G15">
-        <f>AVERAGE(G12:G14)</f>
-        <v>0.99178666666666671</v>
+        <f t="shared" si="1"/>
+        <v>0.99835666666666667</v>
       </c>
       <c r="H15">
-        <f>AVERAGE(H12:H14)</f>
-        <v>0.99074000000000007</v>
-      </c>
-      <c r="I15">
-        <f>AVERAGE(I12:I14)</f>
-        <v>0.8518433333333334</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B29" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="9"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B18" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+    </row>
+    <row r="59" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K59" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="J18:P18"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="A9:I9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="F10:I10"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="B29:I29"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:I7">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11 A16 A14 D14:F14 A12:I13 H14:I14">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:I15">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:I11">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3:I6">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11:I14">
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:I3 A6 A4:B5 D6:E6 D4:F5 H4:I6">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:I6">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1378,13 +2493,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:I15">
+  <conditionalFormatting sqref="B12:I14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -1393,12 +2508,811 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C15F15-AC28-D047-939F-1BBCF0F3A5BE}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:T59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="I15" sqref="G15:I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="13"/>
+      <c r="B2" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="K2" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+    </row>
+    <row r="4" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.94708999999999999</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.96626000000000001</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.96438000000000001</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.94708999999999999</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.96089999999999998</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.95289000000000001</v>
+      </c>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
+    </row>
+    <row r="5" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.99843999999999999</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.99768000000000001</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.99509999999999998</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.98016000000000003</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.99287000000000003</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.99765000000000004</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.99194000000000004</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.97587999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.95660000000000001</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.98846000000000001</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.98309999999999997</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.96416000000000002</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.95043</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.98640000000000005</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.9788</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0.94410000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="8">
+        <f>AVERAGE(C4:C6)</f>
+        <v>0.9777433333333333</v>
+      </c>
+      <c r="D7" s="8">
+        <f>AVERAGE(D4:D6)</f>
+        <v>0.98148666666666662</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" ref="E7:I7" si="0">AVERAGE(E4:E6)</f>
+        <v>0.96956666666666669</v>
+      </c>
+      <c r="G7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.97704666666666673</v>
+      </c>
+      <c r="H7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.97721333333333338</v>
+      </c>
+      <c r="I7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.95762333333333338</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" s="13"/>
+      <c r="B10" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.96147000000000005</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.96377999999999997</v>
+      </c>
+      <c r="E12">
+        <v>0.89551999999999998</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.96147000000000005</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.95472000000000001</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.88058999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.99285000000000001</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.98546</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.96880999999999995</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.92537000000000003</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.99075000000000002</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.98546</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.96477999999999997</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.91044000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.97714000000000001</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.97109999999999996</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.94969000000000003</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.92039000000000004</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.95628999999999997</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.96130000000000004</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0.93359999999999999</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.87063999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <f>AVERAGE(B12:B14)</f>
+        <v>0.98499500000000006</v>
+      </c>
+      <c r="C15">
+        <f>AVERAGE(C12:C14)</f>
+        <v>0.97267666666666663</v>
+      </c>
+      <c r="D15">
+        <f>AVERAGE(D12:D14)</f>
+        <v>0.96075999999999995</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ref="E15:I15" si="1">AVERAGE(E12:E14)</f>
+        <v>0.91375999999999991</v>
+      </c>
+      <c r="F15">
+        <f>AVERAGE(F12:F14)</f>
+        <v>0.97351999999999994</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0.96940999999999999</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>0.95103333333333329</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0.88722333333333336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" s="15"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="15"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A59" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="19"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="19"/>
+      <c r="K59" s="19"/>
+      <c r="L59" s="19"/>
+      <c r="M59" s="19"/>
+      <c r="N59" s="19"/>
+      <c r="O59" s="19"/>
+      <c r="P59" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A59:P59"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="K3:Q3"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:I10"/>
+  </mergeCells>
+  <conditionalFormatting sqref="G7:I7 C7:E7">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K2 A3:I3 F4 A4:A6">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11:I11 A12:A14">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:I15">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:F4 K2 I6">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:F4 K2 I6">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:F4 K2 F6 I6">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:F4 K2 F6:I6">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:I6 K2 E4:F4">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:F12 H14">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:F12 H14">
+    <cfRule type="colorScale" priority="58">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:F12 H14">
+    <cfRule type="colorScale" priority="63">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:F12 H14 F14">
+    <cfRule type="colorScale" priority="69">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:F12 F14:I14">
+    <cfRule type="colorScale" priority="73">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:E11 B14:E14 E12">
+    <cfRule type="colorScale" priority="76">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:I11 B14:I14 E12:F12">
+    <cfRule type="colorScale" priority="79">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:I6 K2 B4:F4">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:I14 B12:F12">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:I4 B6:I6">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:I12 B14:I14">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:I4 B6:I6 C5:E5 G5:I5">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:I12 B14:I14 C13:E13 G13:I13">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:I6">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:I14">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:E14">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:E15">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12:I14">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15:I15">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:E6">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:I6">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:E7">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7:I7">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A20A1141-CC35-C445-9B17-B982DA057CDF}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView zoomScale="165" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:E13"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1407,25 +3321,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
       <c r="P1" s="10"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -1523,13 +3437,13 @@
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
@@ -1624,18 +3538,18 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1729,12 +3643,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C560B6B9-0EFB-1043-93F3-F312679BBBF3}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView zoomScale="165" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView zoomScale="160" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1743,13 +3658,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
@@ -1835,13 +3750,13 @@
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>

</xml_diff>

<commit_message>
Residential feature selection scripts and datata sets generated
</commit_message>
<xml_diff>
--- a/Accuracy Results.xlsx
+++ b/Accuracy Results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Andree/Dropbox/My Mac (Macbooks-MacBook-Pro.local)/Desktop/occupacny_detection/experimentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EAF5D6-A12F-054D-9DF9-153C326DAB6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65912AB-29A9-AA46-9EA0-E19DAC4F4F54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{48E0AA12-B65A-DE4A-8794-21F6F44F596D}"/>
   </bookViews>
@@ -2443,7 +2443,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11 A16 A14 D14:F14 A12:I13 H14:I14">
+  <conditionalFormatting sqref="A16 A11 A14 D14:F14 A12:I13 H14:I14">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2514,7 +2514,7 @@
   <dimension ref="A1:T59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="I15" sqref="G15:I15"/>
+      <selection activeCell="F10" sqref="F10:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3311,8 +3311,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView zoomScale="165" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A2" zoomScale="165" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3649,7 +3649,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:E13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>